<commit_message>
Added interactive gui modality browser
</commit_message>
<xml_diff>
--- a/src/assets/session to file mapping reordered.xlsx
+++ b/src/assets/session to file mapping reordered.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project- Electro\Predict_Social_Behavior\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB480EF-AECE-4AF6-AF8D-EA59360E1DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D76C757-04ED-48F9-B048-C7890AD3BB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36090" yWindow="-14625" windowWidth="26760" windowHeight="14520" xr2:uid="{3085D265-69D8-4F85-99EA-CEE9737561EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3085D265-69D8-4F85-99EA-CEE9737561EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="609">
   <si>
     <t>male</t>
   </si>
@@ -1860,6 +1860,9 @@
   </si>
   <si>
     <t>timestamps</t>
+  </si>
+  <si>
+    <t>no audio</t>
   </si>
 </sst>
 </file>
@@ -1876,12 +1879,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1896,8 +1905,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2238,11 +2248,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFC0B26-DAA0-4CEC-BE28-3292284A2662}">
   <dimension ref="A1:O127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="139.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3323,7 +3336,7 @@
       <c r="H27" t="s">
         <v>9</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="1" t="s">
         <v>138</v>
       </c>
       <c r="K27" t="s">
@@ -3334,6 +3347,9 @@
       </c>
       <c r="N27" t="s">
         <v>141</v>
+      </c>
+      <c r="O27" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -3373,9 +3389,6 @@
       <c r="N28" t="s">
         <v>145</v>
       </c>
-      <c r="O28" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -3399,7 +3412,7 @@
       <c r="H29" t="s">
         <v>9</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="1" t="s">
         <v>146</v>
       </c>
       <c r="K29" t="s">
@@ -3410,6 +3423,9 @@
       </c>
       <c r="N29" t="s">
         <v>149</v>
+      </c>
+      <c r="O29" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -3449,9 +3465,6 @@
       <c r="N30" t="s">
         <v>153</v>
       </c>
-      <c r="O30" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -3475,7 +3488,7 @@
       <c r="H31" t="s">
         <v>9</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="1" t="s">
         <v>154</v>
       </c>
       <c r="K31" t="s">
@@ -3486,6 +3499,9 @@
       </c>
       <c r="N31" t="s">
         <v>157</v>
+      </c>
+      <c r="O31" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>